<commit_message>
Wind Constant in test script lowered. Checked each test for stability
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="flag_test_data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="26">
   <si>
     <t>Test ID</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Average time external force (ms)</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2250,6 +2259,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8A49-4161-B05A-0EBE9494715C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -5494,6 +5508,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B910-4413-ACD1-6C658C4531A6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -9444,6 +9463,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8C2D-47E0-876E-2A6345710250}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -13405,6 +13429,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-03F0-41E1-A83A-4A5542E60B2C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -37519,10 +37548,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -37825,10 +37854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O121"/>
+  <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="S116" sqref="S116"/>
+    <sheetView tabSelected="1" topLeftCell="K88" workbookViewId="0">
+      <selection activeCell="T108" sqref="T108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37837,7 +37866,7 @@
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -37877,8 +37906,11 @@
       <c r="M1" t="s">
         <v>21</v>
       </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -37919,8 +37951,11 @@
         <f>I2-(F2+G2+H2)</f>
         <v>1.076464000000002E-2</v>
       </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -37958,11 +37993,14 @@
         <v>11846</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M66" si="0">I3-(F3+G3+H3)</f>
+        <f t="shared" ref="M3:M61" si="0">I3-(F3+G3+H3)</f>
         <v>2.2441919999999976E-2</v>
       </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -38003,8 +38041,11 @@
         <f t="shared" si="0"/>
         <v>3.3566490000000004E-2</v>
       </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -38045,8 +38086,11 @@
         <f t="shared" si="0"/>
         <v>4.4505240000000001E-2</v>
       </c>
+      <c r="P5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -38087,8 +38131,11 @@
         <f t="shared" si="0"/>
         <v>5.667597000000002E-2</v>
       </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -38129,8 +38176,11 @@
         <f t="shared" si="0"/>
         <v>3.3380900000000047E-2</v>
       </c>
+      <c r="P7" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -38171,8 +38221,11 @@
         <f t="shared" si="0"/>
         <v>4.4717399999999907E-2</v>
       </c>
+      <c r="P8" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -38213,8 +38266,11 @@
         <f t="shared" si="0"/>
         <v>5.6307899999999966E-2</v>
       </c>
+      <c r="P9" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -38255,8 +38311,11 @@
         <f t="shared" si="0"/>
         <v>6.8340199999999962E-2</v>
       </c>
+      <c r="P10" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -38297,8 +38356,11 @@
         <f t="shared" si="0"/>
         <v>8.1505899999999909E-2</v>
       </c>
+      <c r="P11" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -38339,8 +38401,11 @@
         <f t="shared" si="0"/>
         <v>7.0889099999999816E-2</v>
       </c>
+      <c r="P12" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -38381,8 +38446,11 @@
         <f t="shared" si="0"/>
         <v>8.0589500000000314E-2</v>
       </c>
+      <c r="P13" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -38423,8 +38491,11 @@
         <f t="shared" si="0"/>
         <v>9.1884699999999819E-2</v>
       </c>
+      <c r="P14" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -38465,8 +38536,11 @@
         <f t="shared" si="0"/>
         <v>0.10324700000000009</v>
       </c>
+      <c r="P15" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -38507,8 +38581,11 @@
         <f t="shared" si="0"/>
         <v>0.11430449999999981</v>
       </c>
+      <c r="P16" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -38549,8 +38626,11 @@
         <f t="shared" si="0"/>
         <v>0.13287299999999957</v>
       </c>
+      <c r="P17" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -38591,8 +38671,11 @@
         <f t="shared" si="0"/>
         <v>0.14311400000000019</v>
       </c>
+      <c r="P18" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -38633,8 +38716,11 @@
         <f t="shared" si="0"/>
         <v>0.1514120000000001</v>
       </c>
+      <c r="P19" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -38675,8 +38761,11 @@
         <f t="shared" si="0"/>
         <v>0.16701900000000025</v>
       </c>
+      <c r="P20" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -38717,8 +38806,11 @@
         <f t="shared" si="0"/>
         <v>0.17683099999999952</v>
       </c>
+      <c r="P21" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -38759,8 +38851,11 @@
         <f t="shared" si="0"/>
         <v>0.23237900000000078</v>
       </c>
+      <c r="P22" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -38801,8 +38896,11 @@
         <f t="shared" si="0"/>
         <v>0.22652999999999945</v>
       </c>
+      <c r="P23" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -38843,8 +38941,11 @@
         <f t="shared" si="0"/>
         <v>0.2538450000000001</v>
       </c>
+      <c r="P24" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -38885,8 +38986,11 @@
         <f t="shared" si="0"/>
         <v>0.26745199999999958</v>
       </c>
+      <c r="P25" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -38927,8 +39031,11 @@
         <f t="shared" si="0"/>
         <v>0.28862800000000099</v>
       </c>
+      <c r="P26" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -38969,8 +39076,11 @@
         <f t="shared" si="0"/>
         <v>0.45493299999999959</v>
       </c>
+      <c r="P27" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -39011,8 +39121,11 @@
         <f t="shared" si="0"/>
         <v>0.45515399999999939</v>
       </c>
+      <c r="P28" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -39053,8 +39166,11 @@
         <f t="shared" si="0"/>
         <v>0.46205800000000075</v>
       </c>
+      <c r="P29" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -39095,8 +39211,11 @@
         <f t="shared" si="0"/>
         <v>0.48355899999999963</v>
       </c>
+      <c r="P30" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -39137,8 +39256,11 @@
         <f t="shared" si="0"/>
         <v>0.49451300000000042</v>
       </c>
+      <c r="P31" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -39179,8 +39301,11 @@
         <f t="shared" si="0"/>
         <v>1.102299000000001E-2</v>
       </c>
+      <c r="P32" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -39221,8 +39346,11 @@
         <f t="shared" si="0"/>
         <v>2.414007999999998E-2</v>
       </c>
+      <c r="P33" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -39263,8 +39391,11 @@
         <f t="shared" si="0"/>
         <v>3.714307E-2</v>
       </c>
+      <c r="P34" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -39305,8 +39436,11 @@
         <f t="shared" si="0"/>
         <v>4.9755730000000026E-2</v>
       </c>
+      <c r="P35" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -39347,8 +39481,11 @@
         <f t="shared" si="0"/>
         <v>5.9939429999999988E-2</v>
       </c>
+      <c r="P36" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -39389,8 +39526,11 @@
         <f t="shared" si="0"/>
         <v>3.3262600000000031E-2</v>
       </c>
+      <c r="P37" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -39431,8 +39571,11 @@
         <f t="shared" si="0"/>
         <v>4.3993800000000083E-2</v>
       </c>
+      <c r="P38" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -39473,8 +39616,11 @@
         <f t="shared" si="0"/>
         <v>5.7748600000000039E-2</v>
       </c>
+      <c r="P39" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -39515,8 +39661,11 @@
         <f t="shared" si="0"/>
         <v>6.7435499999999982E-2</v>
       </c>
+      <c r="P40" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -39557,8 +39706,11 @@
         <f t="shared" si="0"/>
         <v>8.0984900000000026E-2</v>
       </c>
+      <c r="P41" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -39599,8 +39751,11 @@
         <f t="shared" si="0"/>
         <v>7.0409800000000189E-2</v>
       </c>
+      <c r="P42" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -39641,8 +39796,11 @@
         <f t="shared" si="0"/>
         <v>8.0404800000000165E-2</v>
       </c>
+      <c r="P43" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -39683,8 +39841,11 @@
         <f t="shared" si="0"/>
         <v>9.1221199999999891E-2</v>
       </c>
+      <c r="P44" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -39725,8 +39886,11 @@
         <f t="shared" si="0"/>
         <v>0.1025379999999998</v>
       </c>
+      <c r="P45" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -39767,8 +39931,11 @@
         <f t="shared" si="0"/>
         <v>0.11273270000000002</v>
       </c>
+      <c r="P46" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -39809,8 +39976,11 @@
         <f t="shared" si="0"/>
         <v>0.12660800000000005</v>
       </c>
+      <c r="P47" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -39851,8 +40021,11 @@
         <f t="shared" si="0"/>
         <v>0.13345099999999999</v>
       </c>
+      <c r="P48" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -39893,8 +40066,11 @@
         <f t="shared" si="0"/>
         <v>0.14831199999999978</v>
       </c>
+      <c r="P49" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -39935,8 +40111,11 @@
         <f t="shared" si="0"/>
         <v>0.16243100000000021</v>
       </c>
+      <c r="P50" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -39977,8 +40156,11 @@
         <f t="shared" si="0"/>
         <v>0.17374899999999993</v>
       </c>
+      <c r="P51" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -40019,8 +40201,11 @@
         <f t="shared" si="0"/>
         <v>0.22424399999999967</v>
       </c>
+      <c r="P52" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -40061,8 +40246,11 @@
         <f t="shared" si="0"/>
         <v>0.22408499999999965</v>
       </c>
+      <c r="P53" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -40103,8 +40291,11 @@
         <f t="shared" si="0"/>
         <v>0.25098699999999941</v>
       </c>
+      <c r="P54" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -40145,8 +40336,11 @@
         <f t="shared" si="0"/>
         <v>0.26849800000000013</v>
       </c>
+      <c r="P55" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -40187,8 +40381,11 @@
         <f t="shared" si="0"/>
         <v>0.27973099999999995</v>
       </c>
+      <c r="P56" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -40229,8 +40426,11 @@
         <f t="shared" si="0"/>
         <v>0.45283599999999957</v>
       </c>
+      <c r="P57" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -40271,8 +40471,11 @@
         <f t="shared" si="0"/>
         <v>0.45669000000000004</v>
       </c>
+      <c r="P58" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -40313,8 +40516,11 @@
         <f t="shared" si="0"/>
         <v>0.46324699999999996</v>
       </c>
+      <c r="P59" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -40355,8 +40561,11 @@
         <f t="shared" si="0"/>
         <v>0.48583700000000007</v>
       </c>
+      <c r="P60" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -40397,8 +40606,11 @@
         <f t="shared" si="0"/>
         <v>0.49805899999999959</v>
       </c>
+      <c r="P61" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -40439,8 +40651,11 @@
         <f>I62-H62</f>
         <v>1.8043000000000031E-2</v>
       </c>
+      <c r="P62" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -40481,8 +40696,11 @@
         <f t="shared" ref="M63:M121" si="1">I63-H63</f>
         <v>3.1202999999999981E-2</v>
       </c>
+      <c r="P63" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -40523,8 +40741,11 @@
         <f t="shared" si="1"/>
         <v>4.4294999999999973E-2</v>
       </c>
+      <c r="P64" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -40565,8 +40786,11 @@
         <f t="shared" si="1"/>
         <v>5.5294999999999983E-2</v>
       </c>
+      <c r="P65" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -40607,8 +40831,11 @@
         <f t="shared" si="1"/>
         <v>7.3259999999999992E-2</v>
       </c>
+      <c r="P66" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -40649,8 +40876,11 @@
         <f t="shared" si="1"/>
         <v>6.227000000000027E-2</v>
       </c>
+      <c r="P67" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -40691,8 +40921,11 @@
         <f t="shared" si="1"/>
         <v>6.9450000000000234E-2</v>
       </c>
+      <c r="P68" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -40733,8 +40966,11 @@
         <f t="shared" si="1"/>
         <v>8.2980000000000054E-2</v>
       </c>
+      <c r="P69" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -40775,8 +41011,11 @@
         <f t="shared" si="1"/>
         <v>9.7140000000000004E-2</v>
       </c>
+      <c r="P70" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -40817,8 +41056,11 @@
         <f t="shared" si="1"/>
         <v>0.11047999999999991</v>
       </c>
+      <c r="P71" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -40859,8 +41101,11 @@
         <f t="shared" si="1"/>
         <v>0.16023999999999994</v>
       </c>
+      <c r="P72" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -40901,8 +41146,11 @@
         <f t="shared" si="1"/>
         <v>0.14808999999999983</v>
       </c>
+      <c r="P73" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -40943,8 +41191,11 @@
         <f t="shared" si="1"/>
         <v>0.16542000000000012</v>
       </c>
+      <c r="P74" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -40985,8 +41236,11 @@
         <f t="shared" si="1"/>
         <v>0.18373999999999935</v>
       </c>
+      <c r="P75" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -41027,8 +41281,11 @@
         <f t="shared" si="1"/>
         <v>0.19830000000000059</v>
       </c>
+      <c r="P76" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -41069,8 +41326,11 @@
         <f t="shared" si="1"/>
         <v>0.29300000000000104</v>
       </c>
+      <c r="P77" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -41111,8 +41371,11 @@
         <f t="shared" si="1"/>
         <v>0.2972999999999999</v>
       </c>
+      <c r="P78" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -41153,8 +41416,11 @@
         <f t="shared" si="1"/>
         <v>0.29680000000000106</v>
       </c>
+      <c r="P79" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -41195,8 +41461,11 @@
         <f t="shared" si="1"/>
         <v>0.32349999999999923</v>
       </c>
+      <c r="P80" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -41237,8 +41506,11 @@
         <f t="shared" si="1"/>
         <v>0.36110000000000042</v>
       </c>
+      <c r="P81" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -41279,8 +41551,11 @@
         <f t="shared" si="1"/>
         <v>0.60910000000000153</v>
       </c>
+      <c r="P82" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -41321,8 +41596,11 @@
         <f t="shared" si="1"/>
         <v>0.60430000000000206</v>
       </c>
+      <c r="P83" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -41363,8 +41641,11 @@
         <f t="shared" si="1"/>
         <v>0.6974000000000018</v>
       </c>
+      <c r="P84" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -41405,8 +41686,11 @@
         <f t="shared" si="1"/>
         <v>0.61199999999999832</v>
       </c>
+      <c r="P85" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -41447,8 +41731,11 @@
         <f t="shared" si="1"/>
         <v>0.60440000000000182</v>
       </c>
+      <c r="P86" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -41493,8 +41780,11 @@
         <f>H88-(F88+G88)</f>
         <v>3.2660799999999988</v>
       </c>
+      <c r="P87" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -41535,8 +41825,11 @@
         <f t="shared" si="1"/>
         <v>1.1087000000000025</v>
       </c>
+      <c r="P88" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -41577,8 +41870,11 @@
         <f t="shared" si="1"/>
         <v>1.103900000000003</v>
       </c>
+      <c r="P89" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -41619,8 +41915,11 @@
         <f t="shared" si="1"/>
         <v>1.1092999999999975</v>
       </c>
+      <c r="P90" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -41661,8 +41960,11 @@
         <f t="shared" si="1"/>
         <v>1.1066000000000003</v>
       </c>
+      <c r="P91" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -41703,8 +42005,11 @@
         <f t="shared" si="1"/>
         <v>1.0402000000000022E-2</v>
       </c>
+      <c r="P92" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -41745,8 +42050,11 @@
         <f t="shared" si="1"/>
         <v>2.3655000000000037E-2</v>
       </c>
+      <c r="P93" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -41787,8 +42095,11 @@
         <f t="shared" si="1"/>
         <v>3.5956000000000043E-2</v>
       </c>
+      <c r="P94" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -41829,8 +42140,11 @@
         <f t="shared" si="1"/>
         <v>4.7928000000000026E-2</v>
       </c>
+      <c r="P95" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -41871,8 +42185,11 @@
         <f t="shared" si="1"/>
         <v>6.0709000000000013E-2</v>
       </c>
+      <c r="P96" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -41913,8 +42230,11 @@
         <f t="shared" si="1"/>
         <v>3.2499999999999973E-2</v>
       </c>
+      <c r="P97" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -41955,8 +42275,11 @@
         <f t="shared" si="1"/>
         <v>4.2059999999999986E-2</v>
       </c>
+      <c r="P98" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -41997,8 +42320,11 @@
         <f t="shared" si="1"/>
         <v>5.3329999999999878E-2</v>
       </c>
+      <c r="P99" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -42039,8 +42365,11 @@
         <f t="shared" si="1"/>
         <v>6.8780000000000063E-2</v>
       </c>
+      <c r="P100" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -42081,8 +42410,11 @@
         <f t="shared" si="1"/>
         <v>7.8789999999999916E-2</v>
       </c>
+      <c r="P101" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -42123,8 +42455,11 @@
         <f t="shared" si="1"/>
         <v>7.0699999999999985E-2</v>
       </c>
+      <c r="P102" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -42165,8 +42500,11 @@
         <f t="shared" si="1"/>
         <v>7.6729999999999965E-2</v>
       </c>
+      <c r="P103" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -42207,8 +42545,11 @@
         <f t="shared" si="1"/>
         <v>8.8750000000000107E-2</v>
       </c>
+      <c r="P104" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -42249,8 +42590,11 @@
         <f t="shared" si="1"/>
         <v>0.10084999999999988</v>
       </c>
+      <c r="P105" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -42291,8 +42635,11 @@
         <f t="shared" si="1"/>
         <v>0.10874000000000006</v>
       </c>
+      <c r="P106" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -42333,8 +42680,11 @@
         <f t="shared" si="1"/>
         <v>0.13361999999999963</v>
       </c>
+      <c r="P107" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -42375,8 +42725,11 @@
         <f t="shared" si="1"/>
         <v>0.13398999999999983</v>
       </c>
+      <c r="P108" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -42417,8 +42770,11 @@
         <f t="shared" si="1"/>
         <v>0.14468999999999976</v>
       </c>
+      <c r="P109" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -42459,8 +42815,11 @@
         <f t="shared" si="1"/>
         <v>0.14916000000000018</v>
       </c>
+      <c r="P110" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -42501,8 +42860,11 @@
         <f t="shared" si="1"/>
         <v>0.16959999999999997</v>
       </c>
+      <c r="P111" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -42543,8 +42905,11 @@
         <f t="shared" si="1"/>
         <v>0.2332099999999997</v>
       </c>
+      <c r="P112" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -42585,8 +42950,11 @@
         <f t="shared" si="1"/>
         <v>0.23067000000000171</v>
       </c>
+      <c r="P113" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -42627,8 +42995,11 @@
         <f t="shared" si="1"/>
         <v>0.22975000000000101</v>
       </c>
+      <c r="P114" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -42669,8 +43040,11 @@
         <f t="shared" si="1"/>
         <v>0.24900000000000055</v>
       </c>
+      <c r="P115" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -42714,8 +43088,11 @@
       <c r="O116" t="s">
         <v>15</v>
       </c>
+      <c r="P116" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -42763,8 +43140,11 @@
       <c r="O117" t="s">
         <v>16</v>
       </c>
+      <c r="P117" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -42808,8 +43188,11 @@
       <c r="O118" t="s">
         <v>17</v>
       </c>
+      <c r="P118" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -42853,8 +43236,11 @@
       <c r="O119" t="s">
         <v>18</v>
       </c>
+      <c r="P119" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -42898,8 +43284,11 @@
       <c r="O120" t="s">
         <v>19</v>
       </c>
+      <c r="P120" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -42942,6 +43331,9 @@
       </c>
       <c r="O121" t="s">
         <v>20</v>
+      </c>
+      <c r="P121" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -42999,7 +43391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+    <sheetView topLeftCell="AI1" workbookViewId="0">
       <selection activeCell="BE27" sqref="BE27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Continued work on data analysis chapter
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -37548,10 +37548,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -37856,8 +37856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:XFD121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44306,7 +44306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="AX1" workbookViewId="0">
       <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
@@ -44321,7 +44321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
@@ -44336,7 +44336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
+    <sheetView topLeftCell="AV1" workbookViewId="0">
       <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
@@ -44351,7 +44351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AU1" workbookViewId="0">
       <selection activeCell="AI28" sqref="AI28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished first draft of data analysis chapter. Needs updating with final test results & coefficient values etc. Maybe discussion about anomalies if there are any
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -37856,14 +37856,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:XFD121"/>
+    <sheetView tabSelected="1" topLeftCell="N118" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A91" activeCellId="1" sqref="A62:XFD62 A91:XFD91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -44306,8 +44306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44321,7 +44321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AZ1" workbookViewId="0">
       <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed unstable data from various graphs
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="flag_test_data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="25">
   <si>
     <t>Test ID</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>u</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2664,27 +2661,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$93,flag_test_data!$K$98,flag_test_data!$K$103,flag_test_data!$K$108,flag_test_data!$K$113,flag_test_data!$K$118)</c:f>
+              <c:f>(flag_test_data!$K$93,flag_test_data!$N$93,flag_test_data!$N$94,flag_test_data!$N$95,flag_test_data!$N$97,flag_test_data!$N$96)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12085.65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8824.0950000000012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3750.1983333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>165.96099999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>97.755550000000014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>63.61665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2739,27 +2721,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$94,flag_test_data!$K$99,flag_test_data!$K$104,flag_test_data!$K$109,flag_test_data!$K$114,flag_test_data!$K$119)</c:f>
+              <c:f>(flag_test_data!$K$94,flag_test_data!$N$94,flag_test_data!$N$95,flag_test_data!$N$96,flag_test_data!$N$97,flag_test_data!$N$98)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12647.083333333334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10893.041666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8373.0083333333332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4752.4816666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>134.50549999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65.588883333333342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2814,28 +2781,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$95,flag_test_data!$K$100,flag_test_data!$K$105,flag_test_data!$K$110,flag_test_data!$K$115,flag_test_data!$K$120)</c:f>
+              <c:f>flag_test_data!$N$95:$N$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12843.199999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11628.408333333335</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9882.6183333333338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7427.38</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4221.9866666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.002716666666672</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2863,28 +2812,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$96,flag_test_data!$K$101,flag_test_data!$K$106,flag_test_data!$K$111,flag_test_data!$K$116,flag_test_data!$K$121)</c:f>
+              <c:f>flag_test_data!$N$95:$N$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12959.166666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12177.333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10679.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8772.3283333333329</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6192.1816666666664</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2830.6949999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5890,27 +5821,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$3,flag_test_data!$K$8,flag_test_data!$K$13,flag_test_data!$K$18,flag_test_data!$K$23,flag_test_data!$K$28)</c:f>
+              <c:f>(flag_test_data!$K$3,flag_test_data!$N$2,flag_test_data!$N$3,flag_test_data!$N$4,flag_test_data!$N$5,flag_test_data!$N$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>8572.4849999999988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10980.020000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8351.5666666666657</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4412.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>212.26666666666665</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>123.53616666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5965,7 +5881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$33,flag_test_data!$K$38,flag_test_data!$K$43,flag_test_data!$K$48,flag_test_data!$K$53,flag_test_data!$K$58)</c:f>
+              <c:f>(flag_test_data!$K$33,flag_test_data!$K$38,flag_test_data!$K$43,flag_test_data!$K$48,flag_test_data!$N$40,flag_test_data!$N$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5980,12 +5896,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3574.3683333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>198.29166666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>122.81950000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6040,27 +5950,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$93,flag_test_data!$K$98,flag_test_data!$K$103,flag_test_data!$K$108,flag_test_data!$K$113,flag_test_data!$K$118)</c:f>
+              <c:f>(flag_test_data!$K$93,flag_test_data!$N$93,flag_test_data!$N$94,flag_test_data!$N$95,flag_test_data!$N$96,flag_test_data!$N$97)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12085.65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8824.0950000000012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3750.1983333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>165.96099999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>97.755550000000014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>63.61665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6115,7 +6010,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$63,flag_test_data!$K$68,flag_test_data!$K$73,flag_test_data!$K$78,flag_test_data!$K$83,flag_test_data!$K$88)</c:f>
+              <c:f>(flag_test_data!$K$63,flag_test_data!$K$68,flag_test_data!$K$73,flag_test_data!$N$70,flag_test_data!$N$71,flag_test_data!$N$72)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6127,15 +6022,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>126.43033333333335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75.661100000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48.327750000000009</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31.39661666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6661,7 +6547,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$63,flag_test_data!$K$68,flag_test_data!$K$73,flag_test_data!$K$78,flag_test_data!$K$83,flag_test_data!$K$88)</c:f>
+              <c:f>(flag_test_data!$K$63,flag_test_data!$K$68,flag_test_data!$K$73,flag_test_data!$N$63,flag_test_data!$N$64,flag_test_data!$N$65)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6673,15 +6559,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>126.43033333333335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75.661100000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48.327750000000009</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31.39661666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6736,27 +6613,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$64,flag_test_data!$K$69,flag_test_data!$K$74,flag_test_data!$K$79,flag_test_data!$K$84,flag_test_data!$K$89)</c:f>
+              <c:f>(flag_test_data!$K$64,flag_test_data!$N$64,flag_test_data!$N$65,flag_test_data!$N$66,flag_test_data!$N$67,flag_test_data!$N$68)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>11982.766666666668</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9059.5983333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3536.1549999999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79.022216666666665</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49.086133333333329</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.105550000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6811,27 +6673,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$65,flag_test_data!$K$70,flag_test_data!$K$75,flag_test_data!$K$80,flag_test_data!$K$85,flag_test_data!$K$90)</c:f>
+              <c:f>(flag_test_data!$K$65,flag_test_data!$N$65,flag_test_data!$N$66,flag_test_data!$N$67,flag_test_data!$N$68,flag_test_data!$N$69)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12403.699999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10366.98</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6629.6066666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1491.47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49.816666666666663</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.622199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6860,28 +6707,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$66,flag_test_data!$K$71,flag_test_data!$K$76,flag_test_data!$K$81,flag_test_data!$K$86,flag_test_data!$K$91)</c:f>
+              <c:f>flag_test_data!$N$66:$N$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12597.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11094.641666666668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8248.1283333333322</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4306.53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76.208349999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33.06666666666667</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9966,7 +9795,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$33,flag_test_data!$K$38,flag_test_data!$K$43,flag_test_data!$K$48,flag_test_data!$K$53,flag_test_data!$K$58)</c:f>
+              <c:f>(flag_test_data!$K$33,flag_test_data!$K$38,flag_test_data!$K$43,flag_test_data!$K$48,flag_test_data!$N$33,flag_test_data!$N$34)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -9981,12 +9810,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3574.3683333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>198.29166666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>122.81950000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10041,7 +9864,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$34,flag_test_data!$K$39,flag_test_data!$K$44,flag_test_data!$K$49,flag_test_data!$K$54,flag_test_data!$K$59)</c:f>
+              <c:f>(flag_test_data!$K$34,flag_test_data!$K$39,flag_test_data!$N$37,flag_test_data!$N$38,flag_test_data!$N$39,flag_test_data!$N$40)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10050,18 +9873,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11772.466666666665</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10626.800000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8681.7166666666672</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6144.541666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2375.8066666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10116,27 +9927,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$35,flag_test_data!$K$40,flag_test_data!$K$45,flag_test_data!$K$50,flag_test_data!$K$55,flag_test_data!$K$60)</c:f>
+              <c:f>(flag_test_data!$K$35,flag_test_data!$N$35,flag_test_data!$N$36,flag_test_data!$N$37,flag_test_data!$N$38,flag_test_data!$N$39)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13010.016666666668</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12501.949999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11338.730000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9748.6249999999982</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7351.5449999999992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5194.2833333333328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10165,27 +9961,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$36,flag_test_data!$K$41,flag_test_data!$K$46,flag_test_data!$K$51,flag_test_data!$K$56,flag_test_data!$K$61)</c:f>
+              <c:f>(flag_test_data!$K$36,flag_test_data!$N$36,flag_test_data!$N$37,flag_test_data!$N$38,flag_test_data!$N$39,flag_test_data!$N$40)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13076.800000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12637.933333333332</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11728.700000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10046.571666666665</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7399.8216666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5321.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11602,28 +11383,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$4,flag_test_data!$K$9,flag_test_data!$K$14,flag_test_data!$K$19,flag_test_data!$K$24,flag_test_data!$K$29)</c:f>
+              <c:f>flag_test_data!$N$3:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8765.0516666666663</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12327.683333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10657.685000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8243.0466666666671</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6157.6533333333327</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2409.3416666666667</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11677,7 +11440,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$34,flag_test_data!$K$39,flag_test_data!$K$44,flag_test_data!$K$49,flag_test_data!$K$54,flag_test_data!$K$59)</c:f>
+              <c:f>(flag_test_data!$K$34,flag_test_data!$K$39,flag_test_data!$N$35,flag_test_data!$N$36,flag_test_data!$N$37,flag_test_data!$N$38)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11686,18 +11449,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11772.466666666665</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10626.800000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8681.7166666666672</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6144.541666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2375.8066666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11752,27 +11503,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$94,flag_test_data!$K$99,flag_test_data!$K$104,flag_test_data!$K$109,flag_test_data!$K$114,flag_test_data!$K$119)</c:f>
+              <c:f>(flag_test_data!$K$94,flag_test_data!$N$94,flag_test_data!$N$95,flag_test_data!$N$96,flag_test_data!$N$97,flag_test_data!$N$98)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12647.083333333334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10893.041666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8373.0083333333332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4752.4816666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>134.50549999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65.588883333333342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11827,27 +11563,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$64,flag_test_data!$K$69,flag_test_data!$K$74,flag_test_data!$K$79,flag_test_data!$K$84,flag_test_data!$K$89)</c:f>
+              <c:f>(flag_test_data!$K$64,flag_test_data!$N$64,flag_test_data!$N$65,flag_test_data!$N$66,flag_test_data!$N$67,flag_test_data!$N$68)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>11982.766666666668</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9059.5983333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3536.1549999999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79.022216666666665</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49.086133333333329</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.105550000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13986,7 +13707,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$3,flag_test_data!$K$8,flag_test_data!$K$13,flag_test_data!$K$18,flag_test_data!$K$23,flag_test_data!$K$28)</c:f>
+              <c:f>(flag_test_data!$K$3,flag_test_data!$K$8,flag_test_data!$N$3,flag_test_data!$N$4,flag_test_data!$N$5,flag_test_data!$N$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -13995,18 +13716,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10980.020000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8351.5666666666657</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4412.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>212.26666666666665</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>123.53616666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14061,28 +13770,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$4,flag_test_data!$K$9,flag_test_data!$K$14,flag_test_data!$K$19,flag_test_data!$K$24,flag_test_data!$K$29)</c:f>
+              <c:f>flag_test_data!$N$4:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8765.0516666666663</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12327.683333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10657.685000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8243.0466666666671</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6157.6533333333327</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2409.3416666666667</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14136,28 +13827,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$5,flag_test_data!$K$10,flag_test_data!$K$15,flag_test_data!$K$20,flag_test_data!$K$25,flag_test_data!$K$30)</c:f>
+              <c:f>flag_test_data!$N$5:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8829.2116666666661</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12648.65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11402.904999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9239.1666666666661</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7340.041666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5234.97</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14185,28 +13858,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$6,flag_test_data!$K$11,flag_test_data!$K$16,flag_test_data!$K$21,flag_test_data!$K$26,flag_test_data!$K$31)</c:f>
+              <c:f>flag_test_data!$N$6:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8857.4583333333339</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12796.299999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11821.363333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9461.9583333333339</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7407.1883333333326</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5323.1149999999989</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14660,28 +14315,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$5,flag_test_data!$K$10,flag_test_data!$K$15,flag_test_data!$K$20,flag_test_data!$K$25,flag_test_data!$K$30)</c:f>
+              <c:f>flag_test_data!$N$33:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8829.2116666666661</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12648.65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11402.904999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9239.1666666666661</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7340.041666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5234.97</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14735,27 +14372,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$35,flag_test_data!$K$40,flag_test_data!$K$45,flag_test_data!$K$50,flag_test_data!$K$55,flag_test_data!$K$60)</c:f>
+              <c:f>(flag_test_data!$K$35,flag_test_data!$N$35,flag_test_data!$N$36,flag_test_data!$N$37,flag_test_data!$N$38,flag_test_data!$N$39)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13010.016666666668</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12501.949999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11338.730000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9748.6249999999982</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7351.5449999999992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5194.2833333333328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14810,28 +14432,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$95,flag_test_data!$K$100,flag_test_data!$K$105,flag_test_data!$K$110,flag_test_data!$K$115,flag_test_data!$K$120)</c:f>
+              <c:f>flag_test_data!$N$95:$N$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12843.199999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11628.408333333335</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9882.6183333333338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7427.38</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4221.9866666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.002716666666672</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14885,27 +14489,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$65,flag_test_data!$K$70,flag_test_data!$K$75,flag_test_data!$K$80,flag_test_data!$K$85,flag_test_data!$K$90)</c:f>
+              <c:f>(flag_test_data!$K$65,flag_test_data!$N$65,flag_test_data!$N$66,flag_test_data!$N$67,flag_test_data!$N$68,flag_test_data!$N$70)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12403.699999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10366.98</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6629.6066666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1491.47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49.816666666666663</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.622199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15360,28 +14949,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$6,flag_test_data!$K$11,flag_test_data!$K$16,flag_test_data!$K$21,flag_test_data!$K$26,flag_test_data!$K$31)</c:f>
+              <c:f>flag_test_data!$N$31:$N$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8857.4583333333339</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12796.299999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11821.363333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9461.9583333333339</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7407.1883333333326</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5323.1149999999989</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15435,27 +15006,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$36,flag_test_data!$K$41,flag_test_data!$K$46,flag_test_data!$K$51,flag_test_data!$K$56,flag_test_data!$K$61)</c:f>
+              <c:f>(flag_test_data!$K$36,flag_test_data!$N$36,flag_test_data!$N$37,flag_test_data!$N$38,flag_test_data!$N$39,flag_test_data!$N$40)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13076.800000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12637.933333333332</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11728.700000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10046.571666666665</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7399.8216666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5321.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15510,28 +15066,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$96,flag_test_data!$K$101,flag_test_data!$K$106,flag_test_data!$K$111,flag_test_data!$K$116,flag_test_data!$K$121)</c:f>
+              <c:f>flag_test_data!$N$95:$N$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12959.166666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12177.333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10679.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8772.3283333333329</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6192.1816666666664</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2830.6949999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15585,28 +15123,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$66,flag_test_data!$K$71,flag_test_data!$K$76,flag_test_data!$K$81,flag_test_data!$K$86,flag_test_data!$K$91)</c:f>
+              <c:f>flag_test_data!$N$76:$N$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>12597.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11094.641666666668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8248.1283333333322</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4306.53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76.208349999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33.06666666666667</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -38054,8 +37574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U160" sqref="U160"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R259" sqref="R259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42924,7 +42444,7 @@
         <v>1.2500333333333447E-2</v>
       </c>
       <c r="P92" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q92">
         <f t="shared" si="4"/>
@@ -42977,7 +42497,7 @@
         <v>3.0368999999999979E-2</v>
       </c>
       <c r="P93" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q93">
         <f t="shared" si="4"/>
@@ -43030,7 +42550,7 @@
         <v>5.0657833333333346E-2</v>
       </c>
       <c r="P94" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q94">
         <f t="shared" si="4"/>
@@ -43189,7 +42709,7 @@
         <v>3.275166666666629E-2</v>
       </c>
       <c r="P97" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q97">
         <f t="shared" si="4"/>
@@ -43454,7 +42974,7 @@
         <v>7.3046666666666482E-2</v>
       </c>
       <c r="P102" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q102">
         <f t="shared" si="4"/>
@@ -43719,7 +43239,7 @@
         <v>0.13562499999999922</v>
       </c>
       <c r="P107" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q107">
         <f t="shared" si="4"/>
@@ -44259,7 +43779,7 @@
         <v>16</v>
       </c>
       <c r="P117" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q117">
         <f t="shared" si="4"/>
@@ -44505,7 +44025,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44520,7 +44040,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44535,7 +44055,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44549,7 +44069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Figures updated to reflect graph changes
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="flag_test_data" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Time Step</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Average time calcSpringForce (ms)</t>
   </si>
   <si>
     <t xml:space="preserve"> Average time integrate (ms)</t>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>RK4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average time internal force (ms)</t>
   </si>
 </sst>
 </file>
@@ -2406,7 +2406,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v> Average time calcSpringForce (ms)</c:v>
+                  <c:v> Average time internal force (ms)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v> Average time external force (ms)</c:v>
@@ -5637,7 +5637,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v> Average time calcSpringForce (ms)</c:v>
+                  <c:v> Average time internal force (ms)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v> Average time external force (ms)</c:v>
@@ -9540,7 +9540,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v> Average time calcSpringForce (ms)</c:v>
+                  <c:v> Average time internal force (ms)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v> Average time external force (ms)</c:v>
@@ -13448,7 +13448,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v> Average time calcSpringForce (ms)</c:v>
+                  <c:v> Average time internal force (ms)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v> Average time external force (ms)</c:v>
@@ -37646,8 +37646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K87" activeCellId="17" sqref="F62 I62 K62 F67 I67 K67 F72 I72 K72 F77 I77 K77 F82 I82 K82 F87 I87 K87"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37673,31 +37673,31 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -37705,7 +37705,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -37742,7 +37742,7 @@
         <v>1.2005125000000005E-2</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2">
         <f>I7/I2</f>
@@ -37758,7 +37758,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -37795,7 +37795,7 @@
         <v>2.6516566666666713E-2</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q66" si="1">I8/I3</f>
@@ -37811,7 +37811,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -37848,7 +37848,7 @@
         <v>4.1834231666666638E-2</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
@@ -37864,7 +37864,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>50</v>
@@ -37901,7 +37901,7 @@
         <v>5.7102150000000018E-2</v>
       </c>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
@@ -37917,7 +37917,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -37954,7 +37954,7 @@
         <v>7.3392005000000038E-2</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
@@ -37970,7 +37970,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -38007,7 +38007,7 @@
         <v>3.346506666666671E-2</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
@@ -38023,7 +38023,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -38060,7 +38060,7 @@
         <v>5.055693333333322E-2</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
@@ -38076,7 +38076,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -38113,7 +38113,7 @@
         <v>7.2133716666666903E-2</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
@@ -38129,7 +38129,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -38166,7 +38166,7 @@
         <v>9.3074749999999984E-2</v>
       </c>
       <c r="P10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q10">
         <f t="shared" si="1"/>
@@ -38182,7 +38182,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -38219,7 +38219,7 @@
         <v>0.1181859999999999</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q11">
         <f t="shared" si="1"/>
@@ -38235,7 +38235,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -38272,7 +38272,7 @@
         <v>7.2031033333333161E-2</v>
       </c>
       <c r="P12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q12">
         <f t="shared" si="1"/>
@@ -38288,7 +38288,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>150</v>
@@ -38325,7 +38325,7 @@
         <v>8.7422633333333444E-2</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q13">
         <f t="shared" si="1"/>
@@ -38341,7 +38341,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>150</v>
@@ -38378,7 +38378,7 @@
         <v>0.10755641666666671</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q14">
         <f t="shared" si="1"/>
@@ -38394,7 +38394,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>150</v>
@@ -38431,7 +38431,7 @@
         <v>0.127301316666667</v>
       </c>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q15">
         <f t="shared" si="1"/>
@@ -38447,7 +38447,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>150</v>
@@ -38484,7 +38484,7 @@
         <v>0.14734146666666681</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q16">
         <f t="shared" si="1"/>
@@ -38500,7 +38500,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>200</v>
@@ -38537,7 +38537,7 @@
         <v>0.13208116666666703</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q17">
         <f t="shared" si="1"/>
@@ -38553,7 +38553,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>200</v>
@@ -38590,7 +38590,7 @@
         <v>0.14356333333333282</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q18">
         <f t="shared" si="1"/>
@@ -38606,7 +38606,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>200</v>
@@ -38643,7 +38643,7 @@
         <v>0.1657878333333338</v>
       </c>
       <c r="P19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q19">
         <f t="shared" si="1"/>
@@ -38659,7 +38659,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>200</v>
@@ -38696,7 +38696,7 @@
         <v>0.18480116666666646</v>
       </c>
       <c r="P20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
@@ -38712,7 +38712,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>200</v>
@@ -38749,7 +38749,7 @@
         <v>0.20248633333333244</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21">
         <f t="shared" si="1"/>
@@ -38765,7 +38765,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>250</v>
@@ -38802,7 +38802,7 @@
         <v>0.23667883333333339</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q22">
         <f t="shared" si="1"/>
@@ -38818,7 +38818,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>250</v>
@@ -38855,7 +38855,7 @@
         <v>0.23872766666666756</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q23">
         <f t="shared" si="1"/>
@@ -38871,7 +38871,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>250</v>
@@ -38908,7 +38908,7 @@
         <v>0.26491833333333314</v>
       </c>
       <c r="P24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q24">
         <f t="shared" si="1"/>
@@ -38924,7 +38924,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>250</v>
@@ -38961,7 +38961,7 @@
         <v>0.30442133333333299</v>
       </c>
       <c r="P25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q25">
         <f t="shared" si="1"/>
@@ -38977,7 +38977,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>250</v>
@@ -39014,7 +39014,7 @@
         <v>0.32317666666666689</v>
       </c>
       <c r="P26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q26">
         <f t="shared" si="1"/>
@@ -39030,7 +39030,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>300</v>
@@ -39067,7 +39067,7 @@
         <v>0.46956549999999897</v>
       </c>
       <c r="P27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q27">
         <f t="shared" si="1"/>
@@ -39083,7 +39083,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>300</v>
@@ -39120,7 +39120,7 @@
         <v>0.4668770000000011</v>
       </c>
       <c r="P28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q28">
         <f t="shared" si="1"/>
@@ -39136,7 +39136,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <v>300</v>
@@ -39173,7 +39173,7 @@
         <v>0.48216133333333389</v>
       </c>
       <c r="P29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q29">
         <f t="shared" si="1"/>
@@ -39189,7 +39189,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>300</v>
@@ -39226,7 +39226,7 @@
         <v>0.54561916666666566</v>
       </c>
       <c r="P30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q30">
         <f t="shared" si="1"/>
@@ -39242,7 +39242,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <v>300</v>
@@ -39279,7 +39279,7 @@
         <v>0.57309183333333547</v>
       </c>
       <c r="P31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q31">
         <f t="shared" si="1"/>
@@ -39295,7 +39295,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32">
         <v>50</v>
@@ -39332,7 +39332,7 @@
         <v>1.4851164999999972E-2</v>
       </c>
       <c r="P32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q32">
         <f t="shared" si="1"/>
@@ -39348,7 +39348,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <v>50</v>
@@ -39385,7 +39385,7 @@
         <v>3.121790499999999E-2</v>
       </c>
       <c r="P33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q33">
         <f t="shared" si="1"/>
@@ -39401,7 +39401,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>50</v>
@@ -39438,7 +39438,7 @@
         <v>5.1136891666666656E-2</v>
       </c>
       <c r="P34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q34">
         <f t="shared" si="1"/>
@@ -39454,7 +39454,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35">
         <v>50</v>
@@ -39491,7 +39491,7 @@
         <v>7.123381833333331E-2</v>
       </c>
       <c r="P35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q35">
         <f t="shared" si="1"/>
@@ -39507,7 +39507,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36">
         <v>50</v>
@@ -39544,7 +39544,7 @@
         <v>9.1668359999999977E-2</v>
       </c>
       <c r="P36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q36">
         <f t="shared" si="1"/>
@@ -39560,7 +39560,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37">
         <v>100</v>
@@ -39597,7 +39597,7 @@
         <v>3.3610266666666777E-2</v>
       </c>
       <c r="P37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q37">
         <f t="shared" si="1"/>
@@ -39613,7 +39613,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38">
         <v>100</v>
@@ -39650,7 +39650,7 @@
         <v>5.0109400000000193E-2</v>
       </c>
       <c r="P38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q38">
         <f t="shared" si="1"/>
@@ -39666,7 +39666,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39">
         <v>100</v>
@@ -39703,7 +39703,7 @@
         <v>6.9611449999999908E-2</v>
       </c>
       <c r="P39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q39">
         <f t="shared" si="1"/>
@@ -39719,7 +39719,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -39756,7 +39756,7 @@
         <v>9.2368933333333403E-2</v>
       </c>
       <c r="P40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q40">
         <f t="shared" si="1"/>
@@ -39772,7 +39772,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -39809,7 +39809,7 @@
         <v>0.11595425000000004</v>
       </c>
       <c r="P41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q41">
         <f t="shared" si="1"/>
@@ -39825,7 +39825,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C42">
         <v>150</v>
@@ -39862,7 +39862,7 @@
         <v>7.2854050000000115E-2</v>
       </c>
       <c r="P42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q42">
         <f t="shared" si="1"/>
@@ -39878,7 +39878,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C43">
         <v>150</v>
@@ -39915,7 +39915,7 @@
         <v>8.7226099999999862E-2</v>
       </c>
       <c r="P43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q43">
         <f t="shared" si="1"/>
@@ -39931,7 +39931,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C44">
         <v>150</v>
@@ -39968,7 +39968,7 @@
         <v>0.10776690000000033</v>
       </c>
       <c r="P44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q44">
         <f t="shared" si="1"/>
@@ -39984,7 +39984,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C45">
         <v>150</v>
@@ -40021,7 +40021,7 @@
         <v>0.1281868833333335</v>
       </c>
       <c r="P45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q45">
         <f t="shared" si="1"/>
@@ -40037,7 +40037,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46">
         <v>150</v>
@@ -40074,7 +40074,7 @@
         <v>0.14757719999999952</v>
       </c>
       <c r="P46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q46">
         <f t="shared" si="1"/>
@@ -40090,7 +40090,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C47">
         <v>200</v>
@@ -40127,7 +40127,7 @@
         <v>0.13116866666666738</v>
       </c>
       <c r="P47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q47">
         <f t="shared" si="1"/>
@@ -40143,7 +40143,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C48">
         <v>200</v>
@@ -40180,7 +40180,7 @@
         <v>0.14129649999999927</v>
       </c>
       <c r="P48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q48">
         <f t="shared" si="1"/>
@@ -40196,7 +40196,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49">
         <v>200</v>
@@ -40233,7 +40233,7 @@
         <v>0.16681916666666696</v>
       </c>
       <c r="P49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q49">
         <f t="shared" si="1"/>
@@ -40249,7 +40249,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50">
         <v>200</v>
@@ -40286,7 +40286,7 @@
         <v>0.18733366666666651</v>
       </c>
       <c r="P50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q50">
         <f t="shared" si="1"/>
@@ -40302,7 +40302,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51">
         <v>200</v>
@@ -40339,7 +40339,7 @@
         <v>0.20621433333333261</v>
       </c>
       <c r="P51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q51">
         <f t="shared" si="1"/>
@@ -40355,7 +40355,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52">
         <v>250</v>
@@ -40392,7 +40392,7 @@
         <v>0.23610866666666563</v>
       </c>
       <c r="P52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q52">
         <f t="shared" si="1"/>
@@ -40408,7 +40408,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53">
         <v>250</v>
@@ -40445,7 +40445,7 @@
         <v>0.23703933333333449</v>
       </c>
       <c r="P53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q53">
         <f t="shared" si="1"/>
@@ -40461,7 +40461,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54">
         <v>250</v>
@@ -40498,7 +40498,7 @@
         <v>0.2667465</v>
       </c>
       <c r="P54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q54">
         <f t="shared" si="1"/>
@@ -40514,7 +40514,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55">
         <v>250</v>
@@ -40551,7 +40551,7 @@
         <v>0.30373699999999992</v>
       </c>
       <c r="P55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q55">
         <f t="shared" si="1"/>
@@ -40567,7 +40567,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56">
         <v>250</v>
@@ -40604,7 +40604,7 @@
         <v>0.32346616666666606</v>
       </c>
       <c r="P56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q56">
         <f t="shared" si="1"/>
@@ -40620,7 +40620,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57">
         <v>300</v>
@@ -40657,7 +40657,7 @@
         <v>0.46989700000000045</v>
       </c>
       <c r="P57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q57">
         <f t="shared" si="1"/>
@@ -40673,7 +40673,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58">
         <v>300</v>
@@ -40710,7 +40710,7 @@
         <v>0.46962100000000007</v>
       </c>
       <c r="P58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q58">
         <f t="shared" si="1"/>
@@ -40726,7 +40726,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C59">
         <v>300</v>
@@ -40763,7 +40763,7 @@
         <v>0.48517250000000001</v>
       </c>
       <c r="P59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q59">
         <f t="shared" si="1"/>
@@ -40779,7 +40779,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C60">
         <v>300</v>
@@ -40816,7 +40816,7 @@
         <v>0.53287633333333506</v>
       </c>
       <c r="P60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q60">
         <f t="shared" si="1"/>
@@ -40832,7 +40832,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C61">
         <v>300</v>
@@ -40869,7 +40869,7 @@
         <v>0.57316316666666722</v>
       </c>
       <c r="P61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q61">
         <f t="shared" si="1"/>
@@ -40885,7 +40885,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62">
         <v>50</v>
@@ -40922,7 +40922,7 @@
         <v>1.7698333333333371E-2</v>
       </c>
       <c r="P62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q62">
         <f t="shared" si="1"/>
@@ -40938,7 +40938,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63">
         <v>50</v>
@@ -40975,7 +40975,7 @@
         <v>3.8147500000000112E-2</v>
       </c>
       <c r="P63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q63">
         <f t="shared" si="1"/>
@@ -40991,7 +40991,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C64">
         <v>50</v>
@@ -41028,7 +41028,7 @@
         <v>5.9419333333333491E-2</v>
       </c>
       <c r="P64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q64">
         <f t="shared" si="1"/>
@@ -41044,7 +41044,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65">
         <v>50</v>
@@ -41081,7 +41081,7 @@
         <v>7.9388166666666593E-2</v>
       </c>
       <c r="P65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q65">
         <f t="shared" si="1"/>
@@ -41097,7 +41097,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66">
         <v>50</v>
@@ -41134,7 +41134,7 @@
         <v>0.23834900000000003</v>
       </c>
       <c r="P66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q66">
         <f t="shared" si="1"/>
@@ -41150,7 +41150,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C67">
         <v>100</v>
@@ -41187,7 +41187,7 @@
         <v>6.5544999999999298E-2</v>
       </c>
       <c r="P67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q67">
         <f t="shared" ref="Q67:Q121" si="4">I72/I67</f>
@@ -41203,7 +41203,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68">
         <v>100</v>
@@ -41240,7 +41240,7 @@
         <v>7.8021666666666434E-2</v>
       </c>
       <c r="P68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q68">
         <f t="shared" si="4"/>
@@ -41256,7 +41256,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69">
         <v>100</v>
@@ -41293,7 +41293,7 @@
         <v>0.10259833333333335</v>
       </c>
       <c r="P69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q69">
         <f t="shared" si="4"/>
@@ -41309,7 +41309,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C70">
         <v>100</v>
@@ -41346,7 +41346,7 @@
         <v>0.12297000000000002</v>
       </c>
       <c r="P70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q70">
         <f t="shared" si="4"/>
@@ -41362,7 +41362,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71">
         <v>100</v>
@@ -41399,7 +41399,7 @@
         <v>0.146183333333334</v>
       </c>
       <c r="P71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q71">
         <f t="shared" si="4"/>
@@ -41415,7 +41415,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>150</v>
@@ -41452,7 +41452,7 @@
         <v>0.15761999999999787</v>
       </c>
       <c r="P72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q72">
         <f t="shared" si="4"/>
@@ -41468,7 +41468,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73">
         <v>150</v>
@@ -41505,7 +41505,7 @@
         <v>0.15675499999999953</v>
       </c>
       <c r="P73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q73">
         <f t="shared" si="4"/>
@@ -41521,7 +41521,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C74">
         <v>150</v>
@@ -41558,7 +41558,7 @@
         <v>0.17865000000000109</v>
       </c>
       <c r="P74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q74">
         <f t="shared" si="4"/>
@@ -41574,7 +41574,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75">
         <v>150</v>
@@ -41611,7 +41611,7 @@
         <v>0.20503166666666672</v>
       </c>
       <c r="P75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q75">
         <f t="shared" si="4"/>
@@ -41627,7 +41627,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C76">
         <v>150</v>
@@ -41664,7 +41664,7 @@
         <v>0.23062166666666783</v>
       </c>
       <c r="P76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q76">
         <f t="shared" si="4"/>
@@ -41680,7 +41680,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C77">
         <v>200</v>
@@ -41717,7 +41717,7 @@
         <v>0.30341666666666534</v>
       </c>
       <c r="P77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q77">
         <f t="shared" si="4"/>
@@ -41733,7 +41733,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C78">
         <v>200</v>
@@ -41770,7 +41770,7 @@
         <v>0.30544999999999689</v>
       </c>
       <c r="P78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q78">
         <f t="shared" si="4"/>
@@ -41786,7 +41786,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>200</v>
@@ -41823,7 +41823,7 @@
         <v>0.30809999999999782</v>
       </c>
       <c r="P79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q79">
         <f t="shared" si="4"/>
@@ -41839,7 +41839,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C80">
         <v>200</v>
@@ -41876,7 +41876,7 @@
         <v>0.33963333333333168</v>
       </c>
       <c r="P80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q80">
         <f t="shared" si="4"/>
@@ -41892,7 +41892,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C81">
         <v>200</v>
@@ -41929,7 +41929,7 @@
         <v>0.38261666666666372</v>
       </c>
       <c r="P81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q81">
         <f t="shared" si="4"/>
@@ -41945,7 +41945,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C82">
         <v>250</v>
@@ -41982,7 +41982,7 @@
         <v>0.63016666666666765</v>
       </c>
       <c r="P82" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q82">
         <f t="shared" si="4"/>
@@ -41998,7 +41998,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C83">
         <v>250</v>
@@ -42035,7 +42035,7 @@
         <v>0.61664999999999637</v>
       </c>
       <c r="P83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q83">
         <f t="shared" si="4"/>
@@ -42051,7 +42051,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C84">
         <v>250</v>
@@ -42088,7 +42088,7 @@
         <v>0.62783333333333857</v>
       </c>
       <c r="P84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q84">
         <f t="shared" si="4"/>
@@ -42104,7 +42104,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C85">
         <v>250</v>
@@ -42141,7 +42141,7 @@
         <v>0.61584999999999823</v>
       </c>
       <c r="P85" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q85">
         <f t="shared" si="4"/>
@@ -42157,7 +42157,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C86">
         <v>250</v>
@@ -42194,7 +42194,7 @@
         <v>0.63078333333333347</v>
       </c>
       <c r="P86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q86">
         <f t="shared" si="4"/>
@@ -42210,7 +42210,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C87">
         <v>300</v>
@@ -42251,7 +42251,7 @@
         <v>3.3402266666666556</v>
       </c>
       <c r="P87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q87">
         <f t="shared" si="4"/>
@@ -42267,7 +42267,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C88">
         <v>300</v>
@@ -42304,7 +42304,7 @@
         <v>1.1268333333333409</v>
       </c>
       <c r="P88" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q88">
         <f t="shared" si="4"/>
@@ -42320,7 +42320,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C89">
         <v>300</v>
@@ -42357,7 +42357,7 @@
         <v>1.1288833333333379</v>
       </c>
       <c r="P89" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q89">
         <f t="shared" si="4"/>
@@ -42373,7 +42373,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C90">
         <v>300</v>
@@ -42410,7 +42410,7 @@
         <v>1.1268833333333284</v>
       </c>
       <c r="P90" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q90">
         <f t="shared" si="4"/>
@@ -42426,7 +42426,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C91">
         <v>300</v>
@@ -42463,7 +42463,7 @@
         <v>1.1281333333333272</v>
       </c>
       <c r="P91" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q91">
         <f t="shared" si="4"/>
@@ -42479,7 +42479,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C92">
         <v>50</v>
@@ -42516,7 +42516,7 @@
         <v>1.2500333333333447E-2</v>
       </c>
       <c r="P92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q92">
         <f t="shared" si="4"/>
@@ -42532,7 +42532,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C93">
         <v>50</v>
@@ -42569,7 +42569,7 @@
         <v>3.0368999999999979E-2</v>
       </c>
       <c r="P93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q93">
         <f t="shared" si="4"/>
@@ -42585,7 +42585,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C94">
         <v>50</v>
@@ -42622,7 +42622,7 @@
         <v>5.0657833333333346E-2</v>
       </c>
       <c r="P94" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q94">
         <f t="shared" si="4"/>
@@ -42638,7 +42638,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95">
         <v>50</v>
@@ -42675,7 +42675,7 @@
         <v>7.0892499999999969E-2</v>
       </c>
       <c r="P95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q95">
         <f t="shared" si="4"/>
@@ -42691,7 +42691,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C96">
         <v>50</v>
@@ -42728,7 +42728,7 @@
         <v>9.1197333333333352E-2</v>
       </c>
       <c r="P96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q96">
         <f t="shared" si="4"/>
@@ -42744,7 +42744,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C97">
         <v>100</v>
@@ -42781,7 +42781,7 @@
         <v>3.275166666666629E-2</v>
       </c>
       <c r="P97" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q97">
         <f t="shared" si="4"/>
@@ -42797,7 +42797,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C98">
         <v>100</v>
@@ -42834,7 +42834,7 @@
         <v>4.7579999999999956E-2</v>
       </c>
       <c r="P98" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q98">
         <f t="shared" si="4"/>
@@ -42850,7 +42850,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -42887,7 +42887,7 @@
         <v>6.6791666666666805E-2</v>
       </c>
       <c r="P99" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q99">
         <f t="shared" si="4"/>
@@ -42903,7 +42903,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100">
         <v>100</v>
@@ -42940,7 +42940,7 @@
         <v>8.6811666666666287E-2</v>
       </c>
       <c r="P100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q100">
         <f t="shared" si="4"/>
@@ -42956,7 +42956,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -42993,7 +42993,7 @@
         <v>0.11139999999999972</v>
       </c>
       <c r="P101" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q101">
         <f t="shared" si="4"/>
@@ -43009,7 +43009,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C102">
         <v>150</v>
@@ -43046,7 +43046,7 @@
         <v>7.3046666666666482E-2</v>
       </c>
       <c r="P102" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q102">
         <f t="shared" si="4"/>
@@ -43062,7 +43062,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C103">
         <v>150</v>
@@ -43099,7 +43099,7 @@
         <v>8.0551666666665689E-2</v>
       </c>
       <c r="P103" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q103">
         <f t="shared" si="4"/>
@@ -43115,7 +43115,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C104">
         <v>150</v>
@@ -43152,7 +43152,7 @@
         <v>0.10283166666666688</v>
       </c>
       <c r="P104" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q104">
         <f t="shared" si="4"/>
@@ -43168,7 +43168,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C105">
         <v>150</v>
@@ -43205,7 +43205,7 @@
         <v>0.1214616666666668</v>
       </c>
       <c r="P105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q105">
         <f t="shared" si="4"/>
@@ -43221,7 +43221,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C106">
         <v>150</v>
@@ -43258,7 +43258,7 @@
         <v>0.14204833333333333</v>
       </c>
       <c r="P106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q106">
         <f t="shared" si="4"/>
@@ -43274,7 +43274,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C107">
         <v>200</v>
@@ -43311,7 +43311,7 @@
         <v>0.13562499999999922</v>
       </c>
       <c r="P107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q107">
         <f t="shared" si="4"/>
@@ -43327,7 +43327,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C108">
         <v>200</v>
@@ -43364,7 +43364,7 @@
         <v>0.13536166666666549</v>
       </c>
       <c r="P108" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q108">
         <f t="shared" si="4"/>
@@ -43380,7 +43380,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C109">
         <v>200</v>
@@ -43417,7 +43417,7 @@
         <v>0.15406999999999904</v>
       </c>
       <c r="P109" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q109">
         <f t="shared" si="4"/>
@@ -43433,7 +43433,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C110">
         <v>200</v>
@@ -43470,7 +43470,7 @@
         <v>0.177551666666667</v>
       </c>
       <c r="P110" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q110">
         <f t="shared" si="4"/>
@@ -43486,7 +43486,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C111">
         <v>200</v>
@@ -43523,7 +43523,7 @@
         <v>0.19748333333333346</v>
       </c>
       <c r="P111" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q111">
         <f t="shared" si="4"/>
@@ -43539,7 +43539,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C112">
         <v>250</v>
@@ -43576,7 +43576,7 @@
         <v>0.23816666666666642</v>
       </c>
       <c r="P112" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q112">
         <f t="shared" si="4"/>
@@ -43592,7 +43592,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C113">
         <v>250</v>
@@ -43629,7 +43629,7 @@
         <v>0.24113166666666608</v>
       </c>
       <c r="P113" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q113">
         <f t="shared" si="4"/>
@@ -43645,7 +43645,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C114">
         <v>250</v>
@@ -43682,7 +43682,7 @@
         <v>0.24048666666666563</v>
       </c>
       <c r="P114" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q114">
         <f t="shared" si="4"/>
@@ -43698,7 +43698,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C115">
         <v>250</v>
@@ -43735,7 +43735,7 @@
         <v>0.26753999999999856</v>
       </c>
       <c r="P115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q115">
         <f t="shared" si="4"/>
@@ -43751,7 +43751,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C116">
         <v>250</v>
@@ -43788,10 +43788,10 @@
         <v>0.28651833333333165</v>
       </c>
       <c r="O116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P116" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q116">
         <f t="shared" si="4"/>
@@ -43807,7 +43807,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C117">
         <v>300</v>
@@ -43848,10 +43848,10 @@
         <v>0.84718833333333698</v>
       </c>
       <c r="O117" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q117">
         <f t="shared" si="4"/>
@@ -43867,7 +43867,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C118">
         <v>300</v>
@@ -43904,10 +43904,10 @@
         <v>0.46755000000000102</v>
       </c>
       <c r="O118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P118" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q118">
         <f t="shared" si="4"/>
@@ -43923,7 +43923,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C119">
         <v>300</v>
@@ -43960,10 +43960,10 @@
         <v>0.46809999999999974</v>
       </c>
       <c r="O119" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P119" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q119">
         <f t="shared" si="4"/>
@@ -43979,7 +43979,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C120">
         <v>300</v>
@@ -44016,10 +44016,10 @@
         <v>0.46611666666666629</v>
       </c>
       <c r="O120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P120" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q120">
         <f t="shared" si="4"/>
@@ -44035,7 +44035,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C121">
         <v>300</v>
@@ -44072,10 +44072,10 @@
         <v>0.49076666666666924</v>
       </c>
       <c r="O121" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q121">
         <f t="shared" si="4"/>
@@ -44096,7 +44096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B54" sqref="B54:D59"/>
     </sheetView>
   </sheetViews>
@@ -44110,33 +44110,33 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -44169,7 +44169,7 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3">
         <f>CORREL(A3:A8, D3:D8)</f>
@@ -44206,7 +44206,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4">
         <f>CORREL(E3:E8, H3:H8)</f>
@@ -44273,7 +44273,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6">
         <f>CORREL(A3:A8, B3:B8)</f>
@@ -44310,7 +44310,7 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J7">
         <f>CORREL(E3:E8, F3:F8)</f>
@@ -44349,7 +44349,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9">
         <f>CORREL(A3:A8, C3:C8)</f>
@@ -44358,19 +44358,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
         <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
       </c>
       <c r="J10">
         <f>CORREL(E3:E8, G3:G8)</f>
@@ -44409,7 +44409,7 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12">
         <f>CORREL(A11:A15, B11:B15)</f>
@@ -44432,7 +44432,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J13">
         <f>CORREL(E11:E15, F11:F15)</f>
@@ -44473,33 +44473,33 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>32</v>
-      </c>
-      <c r="H19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -44532,7 +44532,7 @@
         <v>6</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J20">
         <f>CORREL(A20:A25, D20:D25)</f>
@@ -44569,7 +44569,7 @@
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J21">
         <f>CORREL(E20:E25, H20:H25)</f>
@@ -44636,7 +44636,7 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23">
         <f>CORREL(A20:A25, B20:B25)</f>
@@ -44673,7 +44673,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24">
         <f>CORREL(E20:E25, F20:F25)</f>
@@ -44712,7 +44712,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J26">
         <f>CORREL(A20:A25, C20:C25)</f>
@@ -44721,19 +44721,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" t="s">
         <v>41</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" t="s">
-        <v>42</v>
       </c>
       <c r="J27">
         <f>CORREL(E20:E25, G20:G25)</f>
@@ -44772,7 +44772,7 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J29">
         <f>CORREL(A28:A32, B28:B32)</f>
@@ -44795,7 +44795,7 @@
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J30">
         <f>CORREL(E28:E32, F28:F32)</f>
@@ -44836,33 +44836,33 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>27</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>28</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>30</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>31</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>32</v>
-      </c>
-      <c r="H36" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -44895,7 +44895,7 @@
         <v>6</v>
       </c>
       <c r="I37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J37">
         <f>CORREL(A37:A42, D37:D42)</f>
@@ -44932,7 +44932,7 @@
         <v>5</v>
       </c>
       <c r="I38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J38">
         <f>CORREL(E37:E42, H37:H42)</f>
@@ -44999,7 +44999,7 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J40">
         <f>CORREL(A37:A42, B37:B42)</f>
@@ -45036,7 +45036,7 @@
         <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J41">
         <f>CORREL(E37:E42, F37:F42)</f>
@@ -45075,7 +45075,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J43">
         <f>CORREL(A37:A42, C37:C42)</f>
@@ -45084,19 +45084,19 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
         <v>39</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
         <v>40</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" t="s">
         <v>41</v>
-      </c>
-      <c r="F44" t="s">
-        <v>33</v>
-      </c>
-      <c r="I44" t="s">
-        <v>42</v>
       </c>
       <c r="J44">
         <f>CORREL(E37:E42, G37:G42)</f>
@@ -45135,7 +45135,7 @@
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J46">
         <f>CORREL(A45:A49, B45:B49)</f>
@@ -45158,7 +45158,7 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J47">
         <f>CORREL(E45:E49, F45:F49)</f>
@@ -45199,33 +45199,33 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
         <v>26</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>27</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>28</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>29</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>30</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>31</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>32</v>
-      </c>
-      <c r="H53" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -45258,7 +45258,7 @@
         <v>6</v>
       </c>
       <c r="I54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J54">
         <f>CORREL(A54:A59, D54:D59)</f>
@@ -45295,7 +45295,7 @@
         <v>5</v>
       </c>
       <c r="I55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J55">
         <f>CORREL(E54:E59, H54:H59)</f>
@@ -45362,7 +45362,7 @@
         <v>3</v>
       </c>
       <c r="I57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J57">
         <f>CORREL(A54:A59, B54:B59)</f>
@@ -45399,7 +45399,7 @@
         <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J58">
         <f>CORREL(E54:E59, F54:F59)</f>
@@ -45438,7 +45438,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J60">
         <f>CORREL(A54:A59, C54:C59)</f>
@@ -45447,19 +45447,19 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
         <v>39</v>
       </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
         <v>40</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" t="s">
         <v>41</v>
-      </c>
-      <c r="F61" t="s">
-        <v>33</v>
-      </c>
-      <c r="I61" t="s">
-        <v>42</v>
       </c>
       <c r="J61">
         <f>CORREL(E54:E59, G54:G59)</f>
@@ -45498,7 +45498,7 @@
         <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J63">
         <f>CORREL(A62:A66, B62:B66)</f>
@@ -45521,7 +45521,7 @@
         <v>3</v>
       </c>
       <c r="I64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J64">
         <f>CORREL(E62:E66, F62:F66)</f>

</xml_diff>

<commit_message>
Data analysis chapter updated with final test data, correlation coefficients and box plots
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/flag_test_data.xlsx
+++ b/Dissertation_main/Dissertation_main/flag_test_data.xlsx
@@ -5891,12 +5891,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(flag_test_data!$K$3,flag_test_data!$N$2,flag_test_data!$N$3,flag_test_data!$N$4,flag_test_data!$N$5,flag_test_data!$N$6)</c:f>
+              <c:f>(flag_test_data!$K$3,flag_test_data!$K$8,flag_test_data!$N$3,flag_test_data!$N$4,flag_test_data!$N$5,flag_test_data!$N$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>8572.4849999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10980.020000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -37646,8 +37649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S166" sqref="S166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44096,7 +44099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B54" sqref="B54:D59"/>
     </sheetView>
   </sheetViews>
@@ -45599,8 +45602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45614,7 +45617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>

</xml_diff>